<commit_message>
Updates L2/L3 URS and DbLayouts
</commit_message>
<xml_diff>
--- a/DbLayouts/L4-批次作業/InsuOrignal.xlsx
+++ b/DbLayouts/L4-批次作業/InsuOrignal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\SKL\DB\GenTables\L4-批次作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L4-批次作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9132"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -312,12 +312,19 @@
     <t>findOrigInsuNoEq</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>CommericalFlag</t>
+  </si>
+  <si>
+    <t>住宅險改商業險註記</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -395,6 +402,13 @@
       <color theme="1"/>
       <name val="思源宋體"/>
       <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="細明體"/>
+      <family val="3"/>
       <charset val="136"/>
     </font>
   </fonts>
@@ -481,7 +495,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -574,6 +588,9 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -880,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -1260,33 +1277,33 @@
         <v>14</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>49</v>
+        <v>77</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>78</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
+        <v>35</v>
+      </c>
+      <c r="E22" s="24">
+        <v>1</v>
+      </c>
+      <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="19">
         <v>15</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="19">
-        <v>6</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E23" s="19"/>
       <c r="F23" s="19"/>
     </row>
     <row r="24" spans="1:7">
@@ -1294,15 +1311,17 @@
         <v>16</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E24" s="19"/>
+        <v>56</v>
+      </c>
+      <c r="E24" s="19">
+        <v>6</v>
+      </c>
       <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:7">
@@ -1310,18 +1329,34 @@
         <v>17</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="19">
+        <v>18</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C26" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D26" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E26" s="19">
         <v>6</v>
       </c>
-      <c r="F25" s="19"/>
+      <c r="F26" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1343,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>

</xml_diff>